<commit_message>
Update references bibtex and spreadsheet
</commit_message>
<xml_diff>
--- a/01_references/ref_lst.xlsx
+++ b/01_references/ref_lst.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22206"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="204">
   <si>
     <t>Reference Table</t>
   </si>
@@ -571,6 +571,81 @@
   </si>
   <si>
     <t>Helps define bond distance cutoff for Ir-O bonds</t>
+  </si>
+  <si>
+    <t>Python Materials Genomics (pymatgen): A robust, open-source python library for materials analysis</t>
+  </si>
+  <si>
+    <t>Ong, Shyue Ping; Richards, William Davidson; Jain, Anubhav; Hautier, Geoffroy; Kocher, Michael; Cholia, Shreyas; Gunter, Dan; Chevrier, Vincent L.; Persson, Kristin A.; Ceder, Gerbrand</t>
+  </si>
+  <si>
+    <t>https://www-sciencedirect-com.stanford.idm.oclc.org/science/article/pii/S0927025612006295?via%3Dihub</t>
+  </si>
+  <si>
+    <t>Elsevier Computational Materials Science</t>
+  </si>
+  <si>
+    <t>Pymatgen reference</t>
+  </si>
+  <si>
+    <t>Genetic algorithms for computational materials discovery accelerated by machine learning</t>
+  </si>
+  <si>
+    <t>Paul C. Jennings, Steen Lysgaard, Jens Strabo Hummelshøj, Tejs Vegge &amp; Thomas Bligaard</t>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/s41524-019-0181-4</t>
+  </si>
+  <si>
+    <t>Nature Computational Materials</t>
+  </si>
+  <si>
+    <t>Active learning</t>
+  </si>
+  <si>
+    <t>Raman-scattering study of crystallized MF3 compounds (M=Al,Cr,Ga,V,Fe,In): An approach to the short-range-order force constants</t>
+  </si>
+  <si>
+    <t>Daniel, P.; Bulou, A.; Rousseau, M.; Nouet, J.; Leblanc, M.</t>
+  </si>
+  <si>
+    <t>https://journals.aps.org/prb/abstract/10.1103/PhysRevB.42.10545</t>
+  </si>
+  <si>
+    <t>MF3 compounds</t>
+  </si>
+  <si>
+    <t>Thermal expansion and phase transitions of α-AlF3</t>
+  </si>
+  <si>
+    <t>Morelock, Cody R.; Hancock, Justin C.; Wilkinson, Angus P.</t>
+  </si>
+  <si>
+    <t>https://www-sciencedirect-com.stanford.idm.oclc.org/science/article/pii/S0022459614003363</t>
+  </si>
+  <si>
+    <t>Source of alpha-AlF3 phase name</t>
+  </si>
+  <si>
+    <t>Van Den Bossche, Maxime; Grönbeck, Henrik; Hammer, Bjørk</t>
+  </si>
+  <si>
+    <t>https://pubs-acs-org.stanford.idm.oclc.org/doi/full/10.1021/acs.jctc.8b00039</t>
+  </si>
+  <si>
+    <t>J. Chem. Theory Comput</t>
+  </si>
+  <si>
+    <t>Activation of surface oxygen sites on an iridium-based model catalyst for the oxygen evolution reaction</t>
+  </si>
+  <si>
+    <t>Grimaud, Alexis; Demortiere, Arnaud; Saubanere, Matthieu; Dachraoui, Walid; Duchamp, Martial; Doublet, Marie Liesse; Tarascon, Jean Marie</t>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/nenergy2016189</t>
+  </si>
+  <si>
+    <t>Michal gave me this</t>
   </si>
 </sst>
 </file>
@@ -1136,10 +1211,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK56"/>
+  <dimension ref="A1:AMK62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B36" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="J57" sqref="J57"/>
+    <sheetView tabSelected="1" topLeftCell="D38" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2170,6 +2245,135 @@
         <v>178</v>
       </c>
     </row>
+    <row r="57" spans="3:10" ht="15">
+      <c r="C57" s="3">
+        <v>54</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F57" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="H57" s="3">
+        <v>2013</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="58" spans="3:10" ht="15">
+      <c r="C58" s="3">
+        <v>55</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F58" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H58" s="3">
+        <v>2019</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="59" spans="3:10" ht="15">
+      <c r="C59" s="3">
+        <v>56</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F59" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H59" s="3">
+        <v>1990</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="60" spans="3:10" ht="15">
+      <c r="C60" s="3">
+        <v>57</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="F60" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="H60" s="3">
+        <v>2014</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="61" spans="3:10" ht="15">
+      <c r="C61" s="3">
+        <v>58</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="F61" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="H61" s="3">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="62" spans="3:10" ht="15">
+      <c r="C62" s="3">
+        <v>59</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="F62" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="H62" s="3">
+        <v>2017</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F45" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -2181,9 +2385,15 @@
     <hyperlink ref="F54" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="F55" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="F56" r:id="rId9" xr:uid="{61C294A8-93CE-4EB3-B519-F890CA93FE76}"/>
+    <hyperlink ref="F57" r:id="rId10" xr:uid="{991DC90B-7BD6-4ABF-A278-D5A0460EC750}"/>
+    <hyperlink ref="F58" r:id="rId11" xr:uid="{5C6459D1-3533-4F09-BA3D-227972D6CDB6}"/>
+    <hyperlink ref="F59" r:id="rId12" xr:uid="{9D8CE753-06FA-4E18-AFB8-6A8D2AC8DD25}"/>
+    <hyperlink ref="F60" r:id="rId13" xr:uid="{B5FE6781-BC2B-4D3B-ADA1-36DC1BF2624C}"/>
+    <hyperlink ref="F61" r:id="rId14" xr:uid="{B46FD5B6-4681-40D4-A139-049856D80968}"/>
+    <hyperlink ref="F62" r:id="rId15" xr:uid="{21C268F1-45BB-4C97-AC69-12131B7183E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <picture r:id="rId10"/>
+  <picture r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new reference to table
</commit_message>
<xml_diff>
--- a/01_references/ref_lst.xlsx
+++ b/01_references/ref_lst.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="207">
   <si>
     <t>Reference Table</t>
   </si>
@@ -646,6 +646,15 @@
   </si>
   <si>
     <t>Michal gave me this</t>
+  </si>
+  <si>
+    <t>An Atomistic Machine Learning Package for Surface Science and Catalysis</t>
+  </si>
+  <si>
+    <t>Martin Hangaard Hansen, José A. Garrido Torres, Paul C. Jennings, Ziyun Wang, Jacob R. Boes, Osman G. Mamun, Thomas Bligaard</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1904.00904</t>
   </si>
 </sst>
 </file>
@@ -1213,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C33" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2374,9 +2383,21 @@
         <v>203</v>
       </c>
     </row>
-    <row r="63" spans="3:10">
+    <row r="63" spans="3:10" ht="15">
       <c r="C63" s="3">
         <v>60</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="F63" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="H63" s="3">
+        <v>2019</v>
       </c>
     </row>
   </sheetData>
@@ -2396,9 +2417,10 @@
     <hyperlink ref="F60" r:id="rId13" xr:uid="{B5FE6781-BC2B-4D3B-ADA1-36DC1BF2624C}"/>
     <hyperlink ref="F61" r:id="rId14" xr:uid="{B46FD5B6-4681-40D4-A139-049856D80968}"/>
     <hyperlink ref="F62" r:id="rId15" xr:uid="{21C268F1-45BB-4C97-AC69-12131B7183E4}"/>
+    <hyperlink ref="F63" r:id="rId16" xr:uid="{3BC1531C-E56C-4339-A77C-36A89A51D369}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <picture r:id="rId16"/>
+  <picture r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update references, pdf and docx files
</commit_message>
<xml_diff>
--- a/01_references/ref_lst.xlsx
+++ b/01_references/ref_lst.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="247">
   <si>
     <t>Reference Table</t>
   </si>
@@ -763,6 +763,18 @@
   </si>
   <si>
     <t>https://www.nature.com/articles/282281a0</t>
+  </si>
+  <si>
+    <t>Systematic Investigation of Iridium-Based Bimetallic Thin Film Catalysts for the Oxygen Evolution Reaction in Acidic Media</t>
+  </si>
+  <si>
+    <t>Alaina L. StricklerRaul A. FloresLaurie A. KingJens K. NørskovMichal Bajdich*Thomas F. Jaramillo*</t>
+  </si>
+  <si>
+    <t>https://pubs.acs.org/doi/abs/10.1021/acsami.9b13697</t>
+  </si>
+  <si>
+    <t>My doped IrO2 paper</t>
   </si>
 </sst>
 </file>
@@ -1340,10 +1352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK73"/>
+  <dimension ref="A1:AMK74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+      <selection activeCell="J75" sqref="J75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2724,6 +2736,26 @@
       </c>
       <c r="H73" s="3">
         <v>1979</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="15">
+      <c r="C74" s="3">
+        <v>71</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F74" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="H74" s="3">
+        <v>2019</v>
+      </c>
+      <c r="J74" s="3" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -2756,9 +2788,10 @@
     <hyperlink ref="F71" r:id="rId26" xr:uid="{62FAA820-32EA-4255-943E-E779FAD26734}"/>
     <hyperlink ref="F72" r:id="rId27" xr:uid="{DB082187-12BA-4761-8828-97D3C1DDED72}"/>
     <hyperlink ref="F73" r:id="rId28" xr:uid="{AC32DF83-13CC-4DA3-9361-749EA110261E}"/>
+    <hyperlink ref="F74" r:id="rId29" xr:uid="{0B0F8097-BFDD-4A8A-9DC0-697D13A101BD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <picture r:id="rId29"/>
+  <picture r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>